<commit_message>
EM 2d efficiency map added
</commit_message>
<xml_diff>
--- a/SimBAlink_CL/Profile_Generation_Scripts/cellProfile_Calculator.xlsx
+++ b/SimBAlink_CL/Profile_Generation_Scripts/cellProfile_Calculator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="21600" windowHeight="11240"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="21600" windowHeight="11240" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="alphaMask_Calc" sheetId="6" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="OCVcurve_fit" sheetId="8" r:id="rId3"/>
     <sheet name="surfaceArea_Calc" sheetId="4" r:id="rId4"/>
     <sheet name="crp_corner" sheetId="5" r:id="rId5"/>
+    <sheet name="efficiencyMap" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="82">
   <si>
     <t>C</t>
   </si>
@@ -269,6 +270,12 @@
   <si>
     <t>`</t>
   </si>
+  <si>
+    <t>RPM/Torque</t>
+  </si>
+  <si>
+    <t>Scalar Maps</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +284,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,6 +394,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -733,15 +748,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -840,6 +856,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,11 +883,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
+    <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,11 +1169,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1898431664"/>
-        <c:axId val="-1898436016"/>
+        <c:axId val="1153157280"/>
+        <c:axId val="1153148576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1898431664"/>
+        <c:axId val="1153157280"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1"/>
@@ -1199,13 +1231,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1898436016"/>
+        <c:crossAx val="1153148576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1898436016"/>
+        <c:axId val="1153148576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.2"/>
@@ -1264,7 +1296,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1898431664"/>
+        <c:crossAx val="1153157280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2171,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2227,23 +2259,23 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="54"/>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C3" s="37" t="s">
@@ -2758,59 +2790,59 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="45">
-        <f>D4*$C$11</f>
+        <f t="shared" ref="D11:Q11" si="12">D4*$C$11</f>
         <v>0.6</v>
       </c>
       <c r="E11" s="45">
-        <f>E4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
       <c r="F11" s="45">
-        <f>F4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.57499999999999996</v>
       </c>
       <c r="G11" s="45">
-        <f>G4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H11" s="45">
-        <f>H4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="I11" s="45">
-        <f>I4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.52500000000000002</v>
       </c>
       <c r="J11" s="45">
-        <f>J4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="K11" s="45">
-        <f>K4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="L11" s="45">
-        <f>L4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.5</v>
       </c>
       <c r="M11" s="45">
-        <f>M4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.495</v>
       </c>
       <c r="N11" s="45">
-        <f>N4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.48</v>
       </c>
       <c r="O11" s="45">
-        <f>O4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.45500000000000002</v>
       </c>
       <c r="P11" s="45">
-        <f>P4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
       <c r="Q11" s="45">
-        <f>Q4*$C$11</f>
+        <f t="shared" si="12"/>
         <v>0.42499999999999999</v>
       </c>
     </row>
@@ -2959,23 +2991,23 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="49"/>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="55"/>
+      <c r="M19" s="55"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
       <c r="R19" s="49"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
@@ -3033,59 +3065,59 @@
         <v>-5</v>
       </c>
       <c r="D21" s="46">
-        <f>D5*$G$17/$G$16</f>
+        <f t="shared" ref="D21:Q21" si="13">D5*$G$17/$G$16</f>
         <v>2.3519999999999999E-2</v>
       </c>
       <c r="E21" s="46">
-        <f>E5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>2.3519999999999999E-2</v>
       </c>
       <c r="F21" s="46">
-        <f>F5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>2.2539999999999998E-2</v>
       </c>
       <c r="G21" s="46">
-        <f>G5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>2.1560000000000003E-2</v>
       </c>
       <c r="H21" s="46">
-        <f>H5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>2.1560000000000003E-2</v>
       </c>
       <c r="I21" s="46">
-        <f>I5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>2.0580000000000001E-2</v>
       </c>
       <c r="J21" s="46">
-        <f>J5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.9599999999999999E-2</v>
       </c>
       <c r="K21" s="46">
-        <f>K5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.9599999999999999E-2</v>
       </c>
       <c r="L21" s="46">
-        <f>L5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.9599999999999999E-2</v>
       </c>
       <c r="M21" s="46">
-        <f>M5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.9403999999999998E-2</v>
       </c>
       <c r="N21" s="46">
-        <f>N5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.8815999999999999E-2</v>
       </c>
       <c r="O21" s="46">
-        <f>O5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.7836000000000001E-2</v>
       </c>
       <c r="P21" s="46">
-        <f>P5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.7247999999999999E-2</v>
       </c>
       <c r="Q21" s="46">
-        <f>Q5*$G$17/$G$16</f>
+        <f t="shared" si="13"/>
         <v>1.6659999999999998E-2</v>
       </c>
       <c r="R21" s="49"/>
@@ -3096,59 +3128,59 @@
         <v>5</v>
       </c>
       <c r="D22" s="46">
-        <f>D6*$G$17/$G$16</f>
+        <f t="shared" ref="D22:Q22" si="14">D6*$G$17/$G$16</f>
         <v>9.4079999999999997E-3</v>
       </c>
       <c r="E22" s="46">
-        <f>E6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>9.4079999999999997E-3</v>
       </c>
       <c r="F22" s="46">
-        <f>F6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>9.0159999999999997E-3</v>
       </c>
       <c r="G22" s="46">
-        <f>G6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>8.6240000000000015E-3</v>
       </c>
       <c r="H22" s="46">
-        <f>H6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>8.6240000000000015E-3</v>
       </c>
       <c r="I22" s="46">
-        <f>I6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>8.2319999999999997E-3</v>
       </c>
       <c r="J22" s="46">
-        <f>J6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>7.8399999999999997E-3</v>
       </c>
       <c r="K22" s="46">
-        <f>K6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>7.8399999999999997E-3</v>
       </c>
       <c r="L22" s="46">
-        <f>L6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>7.8399999999999997E-3</v>
       </c>
       <c r="M22" s="46">
-        <f>M6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>7.7616000000000004E-3</v>
       </c>
       <c r="N22" s="46">
-        <f>N6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>7.5263999999999999E-3</v>
       </c>
       <c r="O22" s="46">
-        <f>O6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>7.1344000000000008E-3</v>
       </c>
       <c r="P22" s="46">
-        <f>P6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>6.8992000000000003E-3</v>
       </c>
       <c r="Q22" s="46">
-        <f>Q6*$G$17/$G$16</f>
+        <f t="shared" si="14"/>
         <v>6.6640000000000007E-3</v>
       </c>
       <c r="R22" s="49"/>
@@ -3159,59 +3191,59 @@
         <v>15</v>
       </c>
       <c r="D23" s="46">
-        <f>D7*$G$17/$G$16</f>
+        <f t="shared" ref="D23:Q23" si="15">D7*$G$17/$G$16</f>
         <v>7.0559999999999998E-3</v>
       </c>
       <c r="E23" s="46">
-        <f>E7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>7.0559999999999998E-3</v>
       </c>
       <c r="F23" s="46">
-        <f>F7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>6.7619999999999989E-3</v>
       </c>
       <c r="G23" s="46">
-        <f>G7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>6.4679999999999998E-3</v>
       </c>
       <c r="H23" s="46">
-        <f>H7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>6.4679999999999998E-3</v>
       </c>
       <c r="I23" s="46">
-        <f>I7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>6.1739999999999998E-3</v>
       </c>
       <c r="J23" s="46">
-        <f>J7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.8799999999999998E-3</v>
       </c>
       <c r="K23" s="46">
-        <f>K7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.8799999999999998E-3</v>
       </c>
       <c r="L23" s="46">
-        <f>L7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.8799999999999998E-3</v>
       </c>
       <c r="M23" s="46">
-        <f>M7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.8211999999999995E-3</v>
       </c>
       <c r="N23" s="46">
-        <f>N7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.6447999999999993E-3</v>
       </c>
       <c r="O23" s="46">
-        <f>O7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.3508000000000002E-3</v>
       </c>
       <c r="P23" s="46">
-        <f>P7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>5.1744E-3</v>
       </c>
       <c r="Q23" s="46">
-        <f>Q7*$G$17/$G$16</f>
+        <f t="shared" si="15"/>
         <v>4.9979999999999998E-3</v>
       </c>
       <c r="R23" s="49"/>
@@ -3222,59 +3254,59 @@
         <v>25</v>
       </c>
       <c r="D24" s="46">
-        <f>D8*$G$17/$G$16</f>
+        <f t="shared" ref="D24:Q24" si="16">D8*$G$17/$G$16</f>
         <v>5.8799999999999998E-3</v>
       </c>
       <c r="E24" s="46">
-        <f>E8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>5.8799999999999998E-3</v>
       </c>
       <c r="F24" s="46">
-        <f>F8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>5.6349999999999994E-3</v>
       </c>
       <c r="G24" s="46">
-        <f>G8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>5.3900000000000007E-3</v>
       </c>
       <c r="H24" s="46">
-        <f>H8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>5.3900000000000007E-3</v>
       </c>
       <c r="I24" s="46">
-        <f>I8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>5.1450000000000003E-3</v>
       </c>
       <c r="J24" s="46">
-        <f>J8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="K24" s="46">
-        <f>K8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="L24" s="46">
-        <f>L8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="M24" s="46">
-        <f>M8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.8509999999999994E-3</v>
       </c>
       <c r="N24" s="46">
-        <f>N8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.7039999999999998E-3</v>
       </c>
       <c r="O24" s="46">
-        <f>O8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.4590000000000003E-3</v>
       </c>
       <c r="P24" s="46">
-        <f>P8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.3119999999999999E-3</v>
       </c>
       <c r="Q24" s="46">
-        <f>Q8*$G$17/$G$16</f>
+        <f t="shared" si="16"/>
         <v>4.1649999999999994E-3</v>
       </c>
       <c r="R24" s="49"/>
@@ -3285,59 +3317,59 @@
         <v>35</v>
       </c>
       <c r="D25" s="46">
-        <f>D9*$G$17/$G$16</f>
+        <f t="shared" ref="D25:Q25" si="17">D9*$G$17/$G$16</f>
         <v>4.9979999999999998E-3</v>
       </c>
       <c r="E25" s="46">
-        <f>E9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.9979999999999998E-3</v>
       </c>
       <c r="F25" s="46">
-        <f>F9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.7897499999999997E-3</v>
       </c>
       <c r="G25" s="46">
-        <f>G9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.5815000000000005E-3</v>
       </c>
       <c r="H25" s="46">
-        <f>H9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.5815000000000005E-3</v>
       </c>
       <c r="I25" s="46">
-        <f>I9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.3732499999999995E-3</v>
       </c>
       <c r="J25" s="46">
-        <f>J9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.1649999999999994E-3</v>
       </c>
       <c r="K25" s="46">
-        <f>K9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.1649999999999994E-3</v>
       </c>
       <c r="L25" s="46">
-        <f>L9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.1649999999999994E-3</v>
       </c>
       <c r="M25" s="46">
-        <f>M9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>4.1233499999999996E-3</v>
       </c>
       <c r="N25" s="46">
-        <f>N9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>3.9984E-3</v>
       </c>
       <c r="O25" s="46">
-        <f>O9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>3.7901499999999995E-3</v>
       </c>
       <c r="P25" s="46">
-        <f>P9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>3.6652E-3</v>
       </c>
       <c r="Q25" s="46">
-        <f>Q9*$G$17/$G$16</f>
+        <f t="shared" si="17"/>
         <v>3.5402499999999996E-3</v>
       </c>
       <c r="R25" s="49"/>
@@ -3348,59 +3380,59 @@
         <v>45</v>
       </c>
       <c r="D26" s="46">
-        <f>D10*$G$17/$G$16</f>
+        <f t="shared" ref="D26:Q26" si="18">D10*$G$17/$G$16</f>
         <v>3.8219999999999999E-3</v>
       </c>
       <c r="E26" s="46">
-        <f>E10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.8219999999999999E-3</v>
       </c>
       <c r="F26" s="46">
-        <f>F10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.6627499999999998E-3</v>
       </c>
       <c r="G26" s="46">
-        <f>G10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.5035000000000001E-3</v>
       </c>
       <c r="H26" s="46">
-        <f>H10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.5035000000000001E-3</v>
       </c>
       <c r="I26" s="46">
-        <f>I10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.3442500000000004E-3</v>
       </c>
       <c r="J26" s="46">
-        <f>J10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.1849999999999999E-3</v>
       </c>
       <c r="K26" s="46">
-        <f>K10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.1849999999999999E-3</v>
       </c>
       <c r="L26" s="46">
-        <f>L10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.1849999999999999E-3</v>
       </c>
       <c r="M26" s="46">
-        <f>M10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.1531499999999995E-3</v>
       </c>
       <c r="N26" s="46">
-        <f>N10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>3.0575999999999997E-3</v>
       </c>
       <c r="O26" s="46">
-        <f>O10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>2.8983500000000001E-3</v>
       </c>
       <c r="P26" s="46">
-        <f>P10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>2.8028000000000003E-3</v>
       </c>
       <c r="Q26" s="46">
-        <f>Q10*$G$17/$G$16</f>
+        <f t="shared" si="18"/>
         <v>2.70725E-3</v>
       </c>
       <c r="R26" s="49"/>
@@ -3410,59 +3442,59 @@
         <v>55</v>
       </c>
       <c r="D27" s="46">
-        <f>D11*$G$17/$G$16</f>
+        <f t="shared" ref="D27:Q27" si="19">D11*$G$17/$G$16</f>
         <v>2.9399999999999999E-3</v>
       </c>
       <c r="E27" s="46">
-        <f>E11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.9399999999999999E-3</v>
       </c>
       <c r="F27" s="46">
-        <f>F11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.8174999999999997E-3</v>
       </c>
       <c r="G27" s="46">
-        <f>G11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.6950000000000003E-3</v>
       </c>
       <c r="H27" s="46">
-        <f>H11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.6950000000000003E-3</v>
       </c>
       <c r="I27" s="46">
-        <f>I11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.5725000000000001E-3</v>
       </c>
       <c r="J27" s="46">
-        <f>J11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.4499999999999999E-3</v>
       </c>
       <c r="K27" s="46">
-        <f>K11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.4499999999999999E-3</v>
       </c>
       <c r="L27" s="46">
-        <f>L11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.4499999999999999E-3</v>
       </c>
       <c r="M27" s="46">
-        <f>M11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.4254999999999997E-3</v>
       </c>
       <c r="N27" s="46">
-        <f>N11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.3519999999999999E-3</v>
       </c>
       <c r="O27" s="46">
-        <f>O11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.2295000000000001E-3</v>
       </c>
       <c r="P27" s="46">
-        <f>P11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.1559999999999999E-3</v>
       </c>
       <c r="Q27" s="46">
-        <f>Q11*$G$17/$G$16</f>
+        <f t="shared" si="19"/>
         <v>2.0824999999999997E-3</v>
       </c>
     </row>
@@ -3486,7 +3518,7 @@
   <dimension ref="A1:W225"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3509,10 +3541,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="47">
         <v>3.186E-3</v>
       </c>
@@ -3541,11 +3573,11 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
       <c r="F3" t="s">
         <v>20</v>
       </c>
@@ -3584,11 +3616,11 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
       <c r="F7" t="s">
         <v>28</v>
       </c>
@@ -3622,15 +3654,15 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="T10" s="55"/>
-      <c r="U10" s="55"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -3688,11 +3720,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -6807,10 +6839,10 @@
       <c r="C8" s="2">
         <v>3.6074582924435399</v>
       </c>
-      <c r="N8" s="54" t="s">
+      <c r="N8" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="54"/>
+      <c r="O8" s="56"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
@@ -6994,7 +7026,7 @@
       <c r="B24" s="6"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="51" t="s">
         <v>78</v>
       </c>
       <c r="D26" s="49"/>
@@ -7327,11 +7359,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -7371,11 +7403,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -7454,7 +7486,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="H32" sqref="H32:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7866,4 +7898,3550 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.1796875" style="50" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="62" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="D1" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E1" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F1" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="I1" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="J1" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="K1" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="L1" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="M1" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="N1" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="O1" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="P1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="R1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="S1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="T1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="U1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="V1" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="W1" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="X1" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" s="62" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="61">
+        <v>0</v>
+      </c>
+      <c r="D2" s="61">
+        <f>C2+250</f>
+        <v>250</v>
+      </c>
+      <c r="E2" s="61">
+        <f t="shared" ref="E2:AI2" si="0">D2+250</f>
+        <v>500</v>
+      </c>
+      <c r="F2" s="61">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="G2" s="61">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="H2" s="61">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="I2" s="61">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="J2" s="61">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+      <c r="K2" s="61">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="L2" s="61">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="M2" s="61">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="N2" s="61">
+        <f t="shared" si="0"/>
+        <v>2750</v>
+      </c>
+      <c r="O2" s="61">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="P2" s="61">
+        <f t="shared" si="0"/>
+        <v>3250</v>
+      </c>
+      <c r="Q2" s="61">
+        <f t="shared" si="0"/>
+        <v>3500</v>
+      </c>
+      <c r="R2" s="61">
+        <f t="shared" si="0"/>
+        <v>3750</v>
+      </c>
+      <c r="S2" s="61">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+      <c r="T2" s="61">
+        <f t="shared" si="0"/>
+        <v>4250</v>
+      </c>
+      <c r="U2" s="61">
+        <f>T2+250</f>
+        <v>4500</v>
+      </c>
+      <c r="V2" s="61">
+        <f t="shared" si="0"/>
+        <v>4750</v>
+      </c>
+      <c r="W2" s="61">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="X2" s="61">
+        <f t="shared" si="0"/>
+        <v>5250</v>
+      </c>
+      <c r="Y2" s="61">
+        <f t="shared" si="0"/>
+        <v>5500</v>
+      </c>
+      <c r="Z2" s="61">
+        <f t="shared" si="0"/>
+        <v>5750</v>
+      </c>
+      <c r="AA2" s="61">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="AB2" s="61">
+        <f t="shared" si="0"/>
+        <v>6250</v>
+      </c>
+      <c r="AC2" s="61">
+        <f t="shared" si="0"/>
+        <v>6500</v>
+      </c>
+      <c r="AD2" s="61">
+        <f t="shared" si="0"/>
+        <v>6750</v>
+      </c>
+      <c r="AE2" s="61">
+        <f t="shared" si="0"/>
+        <v>7000</v>
+      </c>
+      <c r="AF2" s="61">
+        <f t="shared" si="0"/>
+        <v>7250</v>
+      </c>
+      <c r="AG2" s="61">
+        <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+      <c r="AH2" s="61">
+        <f t="shared" si="0"/>
+        <v>7750</v>
+      </c>
+      <c r="AI2" s="61">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="B3" s="61">
+        <v>0</v>
+      </c>
+      <c r="C3" s="64">
+        <f>$A$3*C1</f>
+        <v>0.75680000000000003</v>
+      </c>
+      <c r="D3" s="64">
+        <f t="shared" ref="D3:AI3" si="1">$A$3*D1</f>
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="E3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="F3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.79120000000000001</v>
+      </c>
+      <c r="G3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="H3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="I3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="J3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8256</v>
+      </c>
+      <c r="K3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8256</v>
+      </c>
+      <c r="L3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8256</v>
+      </c>
+      <c r="M3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8256</v>
+      </c>
+      <c r="N3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="O3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="P3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="Q3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="R3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="S3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="T3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="U3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="V3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="W3" s="64">
+        <f t="shared" si="1"/>
+        <v>0.79120000000000001</v>
+      </c>
+      <c r="X3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="B4" s="61">
+        <f>B3+50</f>
+        <v>50</v>
+      </c>
+      <c r="C4" s="64">
+        <f>$A$4*C1</f>
+        <v>0.75680000000000003</v>
+      </c>
+      <c r="D4" s="64">
+        <f t="shared" ref="D4:AI4" si="2">$A$4*D1</f>
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="E4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="F4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.79120000000000001</v>
+      </c>
+      <c r="G4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="H4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="I4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="J4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8256</v>
+      </c>
+      <c r="K4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8256</v>
+      </c>
+      <c r="L4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8256</v>
+      </c>
+      <c r="M4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8256</v>
+      </c>
+      <c r="N4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="O4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="P4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="Q4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="R4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="S4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="T4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="U4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="V4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.8083999999999999</v>
+      </c>
+      <c r="W4" s="64">
+        <f t="shared" si="2"/>
+        <v>0.79120000000000001</v>
+      </c>
+      <c r="X4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="B5" s="61">
+        <f t="shared" ref="B5:B13" si="3">B4+50</f>
+        <v>100</v>
+      </c>
+      <c r="C5" s="64">
+        <f>$A$5*C1</f>
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="D5" s="64">
+        <f t="shared" ref="D5:AI5" si="4">$A$5*D1</f>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="E5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="F5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="G5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="H5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="I5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.874</v>
+      </c>
+      <c r="J5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="K5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="L5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="M5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="N5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.874</v>
+      </c>
+      <c r="O5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.874</v>
+      </c>
+      <c r="P5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="Q5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="R5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="S5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="T5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="U5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="V5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="W5" s="64">
+        <f t="shared" si="4"/>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="X5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Z5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AC5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AD5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AE5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="64">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="B6" s="61">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="C6" s="64">
+        <f>$A$6*C1</f>
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="D6" s="64">
+        <f t="shared" ref="D6:AI6" si="5">$A$6*D1</f>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="E6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="F6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="G6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="H6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="I6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.874</v>
+      </c>
+      <c r="J6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="K6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="L6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="M6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="N6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.874</v>
+      </c>
+      <c r="O6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.874</v>
+      </c>
+      <c r="P6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="Q6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="R6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="S6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="T6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="U6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="V6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="W6" s="64">
+        <f t="shared" si="5"/>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="X6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Z6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AI6" s="64">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="B7" s="61">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="C7" s="64">
+        <f>$A$7*C1</f>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="D7" s="64">
+        <f t="shared" ref="D7:AI7" si="6">$A$7*D1</f>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="E7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="F7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.874</v>
+      </c>
+      <c r="G7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="H7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="I7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="J7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="K7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="L7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="M7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="N7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="O7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="P7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="Q7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="R7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="S7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="T7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="U7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="V7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="W7" s="64">
+        <f t="shared" si="6"/>
+        <v>0.874</v>
+      </c>
+      <c r="X7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Z7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="64">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="B8" s="61">
+        <f t="shared" si="3"/>
+        <v>250</v>
+      </c>
+      <c r="C8" s="64">
+        <f>$A$8*C1</f>
+        <v>0.8448</v>
+      </c>
+      <c r="D8" s="64">
+        <f t="shared" ref="D8:AI8" si="7">$A$8*D1</f>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="E8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="F8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="G8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="H8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="I8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="J8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.92159999999999997</v>
+      </c>
+      <c r="K8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.92159999999999997</v>
+      </c>
+      <c r="L8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.92159999999999997</v>
+      </c>
+      <c r="M8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.92159999999999997</v>
+      </c>
+      <c r="N8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="O8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="P8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="Q8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="R8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="S8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="T8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="U8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="V8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="W8" s="64">
+        <f t="shared" si="7"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="X8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="64">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="B9" s="61">
+        <f t="shared" si="3"/>
+        <v>300</v>
+      </c>
+      <c r="C9" s="64">
+        <f>$A$9*C1</f>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="D9" s="64">
+        <f t="shared" ref="D9:AI9" si="8">$A$9*D1</f>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="E9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="F9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.874</v>
+      </c>
+      <c r="G9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="H9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="I9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="J9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="K9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="L9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="M9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="N9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="O9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.90249999999999997</v>
+      </c>
+      <c r="P9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="Q9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="R9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="S9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="T9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="U9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="V9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="W9" s="64">
+        <f t="shared" si="8"/>
+        <v>0.874</v>
+      </c>
+      <c r="X9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AG9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="64">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="B10" s="61">
+        <f t="shared" si="3"/>
+        <v>350</v>
+      </c>
+      <c r="C10" s="64">
+        <f>$A$10*C1</f>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="D10" s="64">
+        <f t="shared" ref="D10:AI10" si="9">$A$10*D1</f>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="E10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="F10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="G10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="H10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="I10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="J10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="K10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="L10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="M10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.90239999999999987</v>
+      </c>
+      <c r="N10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="O10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.8929999999999999</v>
+      </c>
+      <c r="P10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="Q10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="R10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="S10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="T10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="U10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="V10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.88359999999999994</v>
+      </c>
+      <c r="W10" s="64">
+        <f t="shared" si="9"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="X10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AH10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="B11" s="61">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+      <c r="C11" s="64">
+        <f>$A$11*C1</f>
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="D11" s="64">
+        <f t="shared" ref="D11:AI11" si="10">$A$11*D1</f>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="E11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="F11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="G11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="H11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="I11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.874</v>
+      </c>
+      <c r="J11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="K11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="L11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="M11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="N11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.874</v>
+      </c>
+      <c r="O11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.874</v>
+      </c>
+      <c r="P11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="Q11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="R11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="S11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="T11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="U11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="V11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="W11" s="64">
+        <f t="shared" si="10"/>
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="X11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Z11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AC11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AE11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="64">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="B12" s="61">
+        <f t="shared" si="3"/>
+        <v>450</v>
+      </c>
+      <c r="C12" s="64">
+        <f>$A$12*C1</f>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="D12" s="64">
+        <f t="shared" ref="D12:AI12" si="11">$A$12*D1</f>
+        <v>0.81</v>
+      </c>
+      <c r="E12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.81</v>
+      </c>
+      <c r="F12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="G12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="H12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="K12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="L12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="M12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="N12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="O12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="P12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="Q12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="R12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="S12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="T12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="U12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="V12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="W12" s="64">
+        <f t="shared" si="11"/>
+        <v>0.82800000000000007</v>
+      </c>
+      <c r="X12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AB12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AC12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AE12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AG12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="64">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>0.88</v>
+      </c>
+      <c r="B13" s="61">
+        <f t="shared" si="3"/>
+        <v>500</v>
+      </c>
+      <c r="C13" s="64">
+        <f>$A$13*C1</f>
+        <v>0.77439999999999998</v>
+      </c>
+      <c r="D13" s="64">
+        <f t="shared" ref="D13:AI13" si="12">$A$13*D1</f>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="E13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="G13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="H13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="I13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="J13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.8448</v>
+      </c>
+      <c r="K13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.8448</v>
+      </c>
+      <c r="L13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.8448</v>
+      </c>
+      <c r="M13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.8448</v>
+      </c>
+      <c r="N13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="O13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="P13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="Q13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="R13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="S13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="T13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="U13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="V13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.82719999999999994</v>
+      </c>
+      <c r="W13" s="64">
+        <f t="shared" si="12"/>
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="X13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Z13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AB13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AC13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AD13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AE13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="64">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="B15" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="66">
+        <v>0</v>
+      </c>
+      <c r="D15" s="66">
+        <f>C15+250</f>
+        <v>250</v>
+      </c>
+      <c r="E15" s="66">
+        <f t="shared" ref="E15:AI15" si="13">D15+250</f>
+        <v>500</v>
+      </c>
+      <c r="F15" s="66">
+        <f t="shared" si="13"/>
+        <v>750</v>
+      </c>
+      <c r="G15" s="66">
+        <f t="shared" si="13"/>
+        <v>1000</v>
+      </c>
+      <c r="H15" s="66">
+        <f t="shared" si="13"/>
+        <v>1250</v>
+      </c>
+      <c r="I15" s="66">
+        <f t="shared" si="13"/>
+        <v>1500</v>
+      </c>
+      <c r="J15" s="66">
+        <f t="shared" si="13"/>
+        <v>1750</v>
+      </c>
+      <c r="K15" s="66">
+        <f t="shared" si="13"/>
+        <v>2000</v>
+      </c>
+      <c r="L15" s="66">
+        <f t="shared" si="13"/>
+        <v>2250</v>
+      </c>
+      <c r="M15" s="66">
+        <f t="shared" si="13"/>
+        <v>2500</v>
+      </c>
+      <c r="N15" s="66">
+        <f t="shared" si="13"/>
+        <v>2750</v>
+      </c>
+      <c r="O15" s="66">
+        <f t="shared" si="13"/>
+        <v>3000</v>
+      </c>
+      <c r="P15" s="66">
+        <f t="shared" si="13"/>
+        <v>3250</v>
+      </c>
+      <c r="Q15" s="66">
+        <f t="shared" si="13"/>
+        <v>3500</v>
+      </c>
+      <c r="R15" s="66">
+        <f t="shared" si="13"/>
+        <v>3750</v>
+      </c>
+      <c r="S15" s="66">
+        <f t="shared" si="13"/>
+        <v>4000</v>
+      </c>
+      <c r="T15" s="66">
+        <f t="shared" si="13"/>
+        <v>4250</v>
+      </c>
+      <c r="U15" s="66">
+        <f>T15+250</f>
+        <v>4500</v>
+      </c>
+      <c r="V15" s="66">
+        <f t="shared" ref="V15:AI15" si="14">U15+250</f>
+        <v>4750</v>
+      </c>
+      <c r="W15" s="66">
+        <f t="shared" si="14"/>
+        <v>5000</v>
+      </c>
+      <c r="X15" s="66">
+        <f t="shared" si="14"/>
+        <v>5250</v>
+      </c>
+      <c r="Y15" s="66">
+        <f t="shared" si="14"/>
+        <v>5500</v>
+      </c>
+      <c r="Z15" s="66">
+        <f t="shared" si="14"/>
+        <v>5750</v>
+      </c>
+      <c r="AA15" s="66">
+        <f t="shared" si="14"/>
+        <v>6000</v>
+      </c>
+      <c r="AB15" s="66">
+        <f t="shared" si="14"/>
+        <v>6250</v>
+      </c>
+      <c r="AC15" s="66">
+        <f t="shared" si="14"/>
+        <v>6500</v>
+      </c>
+      <c r="AD15" s="66">
+        <f t="shared" si="14"/>
+        <v>6750</v>
+      </c>
+      <c r="AE15" s="66">
+        <f t="shared" si="14"/>
+        <v>7000</v>
+      </c>
+      <c r="AF15" s="66">
+        <f t="shared" si="14"/>
+        <v>7250</v>
+      </c>
+      <c r="AG15" s="66">
+        <f t="shared" si="14"/>
+        <v>7500</v>
+      </c>
+      <c r="AH15" s="66">
+        <f t="shared" si="14"/>
+        <v>7750</v>
+      </c>
+      <c r="AI15" s="66">
+        <f t="shared" si="14"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="B16" s="66">
+        <v>0</v>
+      </c>
+      <c r="C16" s="20">
+        <f>(C3/MAX($C$3:$AI$13))*MAX($A$3:$A$13,$C$1:$AI$1)</f>
+        <v>0.78833333333333333</v>
+      </c>
+      <c r="D16" s="20">
+        <f t="shared" ref="D16:AI24" si="15">(D3/MAX($C$3:$AI$13))*MAX($A$3:$A$13,$C$1:$AI$1)</f>
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="F16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.82416666666666671</v>
+      </c>
+      <c r="G16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="H16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="I16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.85104166666666659</v>
+      </c>
+      <c r="J16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86</v>
+      </c>
+      <c r="K16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86</v>
+      </c>
+      <c r="L16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86</v>
+      </c>
+      <c r="M16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86</v>
+      </c>
+      <c r="N16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.85104166666666659</v>
+      </c>
+      <c r="O16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.85104166666666659</v>
+      </c>
+      <c r="P16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="Q16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="R16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="S16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="T16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="U16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="V16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="W16" s="20">
+        <f t="shared" si="15"/>
+        <v>0.82416666666666671</v>
+      </c>
+      <c r="X16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B17" s="66">
+        <f>B16+50</f>
+        <v>50</v>
+      </c>
+      <c r="C17" s="20">
+        <f t="shared" ref="C17:R26" si="16">(C4/MAX($C$3:$AI$13))*MAX($A$3:$A$13,$C$1:$AI$1)</f>
+        <v>0.78833333333333333</v>
+      </c>
+      <c r="D17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="F17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.82416666666666671</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="H17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.85104166666666659</v>
+      </c>
+      <c r="J17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.86</v>
+      </c>
+      <c r="K17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.86</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.86</v>
+      </c>
+      <c r="M17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.86</v>
+      </c>
+      <c r="N17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.85104166666666659</v>
+      </c>
+      <c r="O17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.85104166666666659</v>
+      </c>
+      <c r="P17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="Q17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="R17" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="S17" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="T17" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="U17" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="V17" s="20">
+        <f t="shared" si="15"/>
+        <v>0.84208333333333329</v>
+      </c>
+      <c r="W17" s="20">
+        <f t="shared" si="15"/>
+        <v>0.82416666666666671</v>
+      </c>
+      <c r="X17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B18" s="66">
+        <f t="shared" ref="B18:B26" si="17">B17+50</f>
+        <v>100</v>
+      </c>
+      <c r="C18" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84333333333333327</v>
+      </c>
+      <c r="D18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="F18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88166666666666671</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="H18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="I18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="J18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="K18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="M18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="N18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="O18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="P18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="Q18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="R18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="S18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="T18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="U18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="V18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="W18" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88166666666666671</v>
+      </c>
+      <c r="X18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B19" s="66">
+        <f t="shared" si="17"/>
+        <v>150</v>
+      </c>
+      <c r="C19" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84333333333333327</v>
+      </c>
+      <c r="D19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="F19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88166666666666671</v>
+      </c>
+      <c r="G19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="H19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="I19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="J19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="K19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="M19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="N19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="O19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="P19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="Q19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="R19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="S19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="T19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="U19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="V19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="W19" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88166666666666671</v>
+      </c>
+      <c r="X19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI19" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B20" s="66">
+        <f t="shared" si="17"/>
+        <v>200</v>
+      </c>
+      <c r="C20" s="20">
+        <f t="shared" si="16"/>
+        <v>0.87083333333333335</v>
+      </c>
+      <c r="D20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.890625</v>
+      </c>
+      <c r="E20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.890625</v>
+      </c>
+      <c r="F20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="G20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="H20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="I20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94010416666666652</v>
+      </c>
+      <c r="J20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="K20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="L20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="M20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="N20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94010416666666652</v>
+      </c>
+      <c r="O20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94010416666666652</v>
+      </c>
+      <c r="P20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="Q20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="R20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="S20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="T20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="U20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="V20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="W20" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="X20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI20" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B21" s="66">
+        <f t="shared" si="17"/>
+        <v>250</v>
+      </c>
+      <c r="C21" s="20">
+        <f t="shared" si="16"/>
+        <v>0.88</v>
+      </c>
+      <c r="D21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="E21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="G21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="H21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="I21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="J21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+      <c r="K21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+      <c r="L21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+      <c r="M21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+      <c r="N21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="O21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="P21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="Q21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="R21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="S21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="T21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="U21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="V21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="W21" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="X21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI21" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B22" s="66">
+        <f t="shared" si="17"/>
+        <v>300</v>
+      </c>
+      <c r="C22" s="20">
+        <f t="shared" si="16"/>
+        <v>0.87083333333333335</v>
+      </c>
+      <c r="D22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.890625</v>
+      </c>
+      <c r="E22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.890625</v>
+      </c>
+      <c r="F22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="G22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="H22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="I22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94010416666666652</v>
+      </c>
+      <c r="J22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="K22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="L22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="M22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="N22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94010416666666652</v>
+      </c>
+      <c r="O22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.94010416666666652</v>
+      </c>
+      <c r="P22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="Q22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="R22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="S22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="T22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="U22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="V22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="W22" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="X22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI22" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B23" s="66">
+        <f t="shared" si="17"/>
+        <v>350</v>
+      </c>
+      <c r="C23" s="20">
+        <f t="shared" si="16"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="D23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="E23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="F23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="G23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="H23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="I23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="J23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="K23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="L23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.93999999999999984</v>
+      </c>
+      <c r="N23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="O23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.9302083333333333</v>
+      </c>
+      <c r="P23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="Q23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="R23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="S23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="T23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="U23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="V23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92041666666666655</v>
+      </c>
+      <c r="W23" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="X23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Z23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AA23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AC23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AG23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AH23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AI23" s="20">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B24" s="66">
+        <f t="shared" si="17"/>
+        <v>400</v>
+      </c>
+      <c r="C24" s="20">
+        <f t="shared" si="16"/>
+        <v>0.84333333333333327</v>
+      </c>
+      <c r="D24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="E24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="F24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.88166666666666671</v>
+      </c>
+      <c r="G24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="H24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="I24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="J24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="K24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="L24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="M24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.92</v>
+      </c>
+      <c r="N24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="O24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.91041666666666665</v>
+      </c>
+      <c r="P24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="Q24" s="20">
+        <f t="shared" si="15"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="R24" s="20">
+        <f t="shared" ref="D24:AI26" si="18">(R11/MAX($C$3:$AI$13))*MAX($A$3:$A$13,$C$1:$AI$1)</f>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="S24" s="20">
+        <f t="shared" si="18"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="T24" s="20">
+        <f t="shared" si="18"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="U24" s="20">
+        <f t="shared" si="18"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="V24" s="20">
+        <f t="shared" si="18"/>
+        <v>0.90083333333333337</v>
+      </c>
+      <c r="W24" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88166666666666671</v>
+      </c>
+      <c r="X24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AG24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AI24" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B25" s="66">
+        <f t="shared" si="17"/>
+        <v>450</v>
+      </c>
+      <c r="C25" s="20">
+        <f t="shared" si="16"/>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="D25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.84375000000000011</v>
+      </c>
+      <c r="E25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.84375000000000011</v>
+      </c>
+      <c r="F25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="G25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="H25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="I25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.890625</v>
+      </c>
+      <c r="J25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="K25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="L25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="M25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="N25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.890625</v>
+      </c>
+      <c r="O25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.890625</v>
+      </c>
+      <c r="P25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="Q25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="R25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="S25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="T25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="U25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="V25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88124999999999998</v>
+      </c>
+      <c r="W25" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="X25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AD25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AF25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AG25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AH25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AI25" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="B26" s="66">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="C26" s="20">
+        <f t="shared" si="16"/>
+        <v>0.80666666666666664</v>
+      </c>
+      <c r="D26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="E26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.82500000000000007</v>
+      </c>
+      <c r="F26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.84333333333333327</v>
+      </c>
+      <c r="G26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="H26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="I26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.87083333333333335</v>
+      </c>
+      <c r="J26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88</v>
+      </c>
+      <c r="K26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88</v>
+      </c>
+      <c r="L26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88</v>
+      </c>
+      <c r="M26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.88</v>
+      </c>
+      <c r="N26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.87083333333333335</v>
+      </c>
+      <c r="O26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.87083333333333335</v>
+      </c>
+      <c r="P26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="Q26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="R26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="S26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="T26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="U26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="V26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.86166666666666658</v>
+      </c>
+      <c r="W26" s="20">
+        <f t="shared" si="18"/>
+        <v>0.84333333333333327</v>
+      </c>
+      <c r="X26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="Z26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AF26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AG26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AI26" s="20">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+    </row>
+    <row r="29" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+    </row>
+    <row r="30" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+    </row>
+    <row r="31" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+    </row>
+    <row r="32" spans="2:35" x14ac:dyDescent="0.35">
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>